<commit_message>
add support for date cells
</commit_message>
<xml_diff>
--- a/src/test/resources/excelFile.xlsx
+++ b/src/test/resources/excelFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurent/git/bonita-connector-read-excel/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91306C3A-4AC6-5847-9CB9-CFB2375D40F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F59673F-AD09-BA48-ABC7-53BEB9006D13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="20100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="200" yWindow="460" windowWidth="38400" windowHeight="19500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t/>
   </si>
@@ -52,12 +52,18 @@
   </si>
   <si>
     <t>jack</t>
+  </si>
+  <si>
+    <t>helen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -88,7 +94,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -361,19 +367,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C36E4B6-C4A3-D441-9EB4-DAEA9EA5D267}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.42578125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="22.5703125" style="1" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C1" t="s">
@@ -403,6 +412,17 @@
       </c>
       <c r="C3">
         <v>8652</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
+        <v>25908</v>
+      </c>
+      <c r="C4">
+        <v>6587</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* skip empty lines * add empty columns even if no data is present
</commit_message>
<xml_diff>
--- a/src/test/resources/excelFile.xlsx
+++ b/src/test/resources/excelFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10323"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurent/git/bonita-connector-read-excel/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F59673F-AD09-BA48-ABC7-53BEB9006D13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5DAAE0F-537F-C246-A4F3-6039CE6DC702}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="460" windowWidth="38400" windowHeight="19500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t/>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>helen</t>
+  </si>
+  <si>
+    <t>emptyColumn</t>
   </si>
 </sst>
 </file>
@@ -62,7 +65,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -94,7 +97,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -367,10 +370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C36E4B6-C4A3-D441-9EB4-DAEA9EA5D267}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.42578125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -388,6 +391,9 @@
       <c r="C1" t="s">
         <v>4</v>
       </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -403,25 +409,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1">
-        <v>17782</v>
-      </c>
-      <c r="C3">
-        <v>8652</v>
-      </c>
-    </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>17782</v>
+      </c>
+      <c r="C4">
+        <v>8652</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B5" s="1">
         <v>25908</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>6587</v>
       </c>
     </row>

</xml_diff>